<commit_message>
used barplot for afferent value comparison instead of simple plot with points
</commit_message>
<xml_diff>
--- a/Results/AVP_comparison.xlsx
+++ b/Results/AVP_comparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Fall at OGD beginning</t>
   </si>
@@ -66,19 +66,28 @@
   </si>
   <si>
     <t>very long and smooth line of restoration</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -90,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -124,30 +133,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="16">
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -271,8 +392,47 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -285,16 +445,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:G17" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:G18" totalsRowCount="1" headerRowDxfId="13">
   <autoFilter ref="A1:G17"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" name="Fall at OGD beginning" dataDxfId="5"/>
-    <tableColumn id="3" name="Rise right before SD" dataDxfId="4"/>
-    <tableColumn id="4" name="Fall at SD" dataDxfId="3"/>
-    <tableColumn id="5" name="Restoration" dataDxfId="2"/>
-    <tableColumn id="6" name="SD" dataDxfId="1"/>
-    <tableColumn id="7" name="comment"/>
+    <tableColumn id="1" name="ID" totalsRowLabel="%" dataDxfId="12" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Fall at OGD beginning" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="5">
+      <totalsRowFormula>(SUM(B2:B16)/COUNT(B2:B16))*100</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Rise right before SD" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="4">
+      <totalsRowFormula>(SUM(C2:C16)/COUNT(C2:C16))*100</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Fall at SD" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="3">
+      <totalsRowFormula>(SUM(D2:D16)/COUNT(D2:D16))*100</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Restoration" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="2">
+      <totalsRowFormula>(SUM(E2:E16)/COUNT(E2:E16))*100</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="SD" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="1">
+      <totalsRowFormula>(SUM(F2:F16)/COUNT(F2:F16))*100</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="comment" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,8 +1098,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4">
+        <f>(SUM(B2:B16)/COUNT(B2:B16))*100</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" ref="C18:F18" si="0">(SUM(C2:C16)/COUNT(C2:C16))*100</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>